<commit_message>
docs(sprint): Add sprint 1 backlog tasks
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DECA7E7B-91DF-40CC-B1C9-F971555D4309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85749AC-229F-4004-81EA-B3D05FC98865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHIVE" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Dropdown Keys - DO NOT DELETE" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'RECORD BOOK'!$B$1:$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="76">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -295,12 +295,15 @@
   <si>
     <t>Ettore Farinelli</t>
   </si>
+  <si>
+    <t>Define Backlog for the entire project</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +395,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -605,11 +615,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1113,10 +1123,10 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H50"/>
+  <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1168,7 +1178,7 @@
       <c r="C3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1178,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="22.05" customHeight="1">
@@ -1188,7 +1198,7 @@
       <c r="C4" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1198,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="22.05" customHeight="1">
@@ -1208,7 +1218,7 @@
       <c r="C5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1218,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="22.05" customHeight="1">
@@ -1228,7 +1238,7 @@
       <c r="C6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="30" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1238,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="22.05" customHeight="1">
@@ -1248,7 +1258,7 @@
       <c r="C7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="30" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1258,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="22.05" customHeight="1">
@@ -1268,7 +1278,7 @@
       <c r="C8" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="30" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1278,27 +1288,27 @@
         <v>12</v>
       </c>
       <c r="G8" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="22.05" customHeight="1">
       <c r="B9" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="22.05" customHeight="1">
@@ -1308,11 +1318,11 @@
       <c r="C10" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>35</v>
+      <c r="D10" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>12</v>
@@ -1328,11 +1338,11 @@
       <c r="C11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>45</v>
+      <c r="D11" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>12</v>
@@ -1348,16 +1358,18 @@
       <c r="C12" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>36</v>
+      <c r="D12" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="22.05" customHeight="1">
       <c r="B13" s="17" t="s">
@@ -1366,14 +1378,14 @@
       <c r="C13" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>37</v>
+      <c r="D13" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="12"/>
     </row>
@@ -1384,14 +1396,14 @@
       <c r="C14" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>38</v>
+      <c r="D14" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G14" s="12"/>
     </row>
@@ -1402,11 +1414,11 @@
       <c r="C15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>39</v>
+      <c r="D15" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>12</v>
@@ -1420,11 +1432,11 @@
       <c r="C16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>40</v>
+      <c r="D16" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>12</v>
@@ -1438,14 +1450,14 @@
       <c r="C17" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>41</v>
+      <c r="D17" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="12"/>
     </row>
@@ -1456,11 +1468,11 @@
       <c r="C18" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="29" t="s">
-        <v>42</v>
+      <c r="D18" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>13</v>
@@ -1474,14 +1486,14 @@
       <c r="C19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="29" t="s">
-        <v>43</v>
+      <c r="D19" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G19" s="12"/>
     </row>
@@ -1493,13 +1505,13 @@
         <v>74</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="12"/>
     </row>
@@ -1511,13 +1523,13 @@
         <v>74</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="12"/>
     </row>
@@ -1529,25 +1541,25 @@
         <v>74</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="2:7" ht="22.05" customHeight="1">
       <c r="B23" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>19</v>
@@ -1559,13 +1571,13 @@
     </row>
     <row r="24" spans="2:7" ht="22.05" customHeight="1">
       <c r="B24" s="17" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>19</v>
@@ -1577,13 +1589,13 @@
     </row>
     <row r="25" spans="2:7" ht="22.05" customHeight="1">
       <c r="B25" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>19</v>
@@ -1601,7 +1613,7 @@
         <v>74</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>19</v>
@@ -1619,7 +1631,7 @@
         <v>74</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>19</v>
@@ -1637,7 +1649,7 @@
         <v>74</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>19</v>
@@ -1655,7 +1667,7 @@
         <v>74</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>19</v>
@@ -1673,7 +1685,7 @@
         <v>74</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>19</v>
@@ -1691,7 +1703,7 @@
         <v>74</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>19</v>
@@ -1703,13 +1715,13 @@
     </row>
     <row r="32" spans="2:7" ht="22.05" customHeight="1">
       <c r="B32" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>19</v>
@@ -1721,13 +1733,13 @@
     </row>
     <row r="33" spans="2:7" ht="22.05" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>19</v>
@@ -1745,7 +1757,7 @@
         <v>74</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>19</v>
@@ -1763,13 +1775,13 @@
         <v>74</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="12"/>
     </row>
@@ -1781,49 +1793,49 @@
         <v>74</v>
       </c>
       <c r="D36" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="2:7" ht="22.05" customHeight="1">
+      <c r="B37" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="17" t="s">
+      <c r="E37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="12"/>
-    </row>
-    <row r="37" spans="2:7" ht="21.6" customHeight="1">
-      <c r="B37" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="30" t="s">
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="2:7" ht="21.6" customHeight="1">
+      <c r="B38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="17" t="s">
+      <c r="E38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="2:7" ht="22.05" customHeight="1">
-      <c r="B38" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>13</v>
       </c>
       <c r="G38" s="12"/>
     </row>
@@ -1835,13 +1847,13 @@
         <v>74</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" s="12"/>
     </row>
@@ -1853,31 +1865,31 @@
         <v>74</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="2:7" ht="22.05" customHeight="1">
       <c r="B41" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" s="12"/>
     </row>
@@ -1889,7 +1901,7 @@
         <v>74</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>19</v>
@@ -1901,13 +1913,13 @@
     </row>
     <row r="43" spans="2:7" ht="22.05" customHeight="1">
       <c r="B43" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>19</v>
@@ -1919,13 +1931,13 @@
     </row>
     <row r="44" spans="2:7" ht="22.05" customHeight="1">
       <c r="B44" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>19</v>
@@ -1943,7 +1955,7 @@
         <v>74</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>19</v>
@@ -1955,13 +1967,13 @@
     </row>
     <row r="46" spans="2:7" ht="22.05" customHeight="1">
       <c r="B46" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>19</v>
@@ -1979,7 +1991,7 @@
         <v>74</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>19</v>
@@ -1990,23 +2002,41 @@
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="2:7" ht="22.05" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="16">
-        <f>SUM(G3:G11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" ht="22.05" customHeight="1"/>
-    <row r="50" ht="22.05" customHeight="1"/>
+      <c r="B48" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="2:7" ht="22.05" customHeight="1">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="16">
+        <f>SUM(G3:G12)</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="22.05" customHeight="1"/>
+    <row r="51" spans="2:7" ht="22.05" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B47">
+  <conditionalFormatting sqref="B3:B48">
     <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Update">
       <formula>NOT(ISERROR(SEARCH("Update",B3)))</formula>
     </cfRule>
@@ -2023,7 +2053,7 @@
       <formula>NOT(ISERROR(SEARCH("Research",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E47">
+  <conditionalFormatting sqref="E3:E48">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",E3)))</formula>
     </cfRule>
@@ -2040,7 +2070,7 @@
       <formula>NOT(ISERROR(SEARCH("In Progress",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F47">
+  <conditionalFormatting sqref="F3:F48">
     <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F3)))</formula>
     </cfRule>
@@ -2060,19 +2090,19 @@
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$D$4:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F47</xm:sqref>
+          <xm:sqref>F3:F48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F0F8AA5-B689-4426-BA33-6C1D47615340}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B47</xm:sqref>
+          <xm:sqref>B3:B48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B4C2DC5-C50B-4F79-B003-80EA0FBD9D80}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$F$4:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E47</xm:sqref>
+          <xm:sqref>E3:E48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
refactor(gameloop): Refactor of gameloop to be more idiomatic Scala and backlog update
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85749AC-229F-4004-81EA-B3D05FC98865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F02A4-DEC2-4132-8ED1-7D282C990325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHIVE" sheetId="11" r:id="rId1"/>
@@ -603,6 +603,12 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -614,12 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1125,8 +1125,8 @@
   </sheetPr>
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1144,12 +1144,12 @@
       <c r="B1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="2:8" ht="27" customHeight="1">
       <c r="B2" s="14" t="s">
@@ -1178,7 +1178,7 @@
       <c r="C3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="26" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1188,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="22.05" customHeight="1">
@@ -1198,7 +1198,7 @@
       <c r="C4" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="26" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1208,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="22.05" customHeight="1">
@@ -1218,7 +1218,7 @@
       <c r="C5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1228,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="22.05" customHeight="1">
@@ -1238,7 +1238,7 @@
       <c r="C6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="26" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1248,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="22.05" customHeight="1">
@@ -1258,7 +1258,7 @@
       <c r="C7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1268,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="22.05" customHeight="1">
@@ -1278,7 +1278,7 @@
       <c r="C8" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="26" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="22.05" customHeight="1">
@@ -1298,7 +1298,7 @@
       <c r="C9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="25" t="s">
         <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1318,7 +1318,7 @@
       <c r="C10" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1328,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="22.05" customHeight="1">
@@ -1338,7 +1338,7 @@
       <c r="C11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1348,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="22.05" customHeight="1">
@@ -1358,7 +1358,7 @@
       <c r="C12" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1368,7 +1368,7 @@
         <v>12</v>
       </c>
       <c r="G12" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="22.05" customHeight="1">
@@ -1378,7 +1378,7 @@
       <c r="C13" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="26" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1387,7 +1387,9 @@
       <c r="F13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="22.05" customHeight="1">
       <c r="B14" s="17" t="s">
@@ -1396,7 +1398,7 @@
       <c r="C14" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="26" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1405,7 +1407,9 @@
       <c r="F14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="22.05" customHeight="1">
       <c r="B15" s="17" t="s">
@@ -1414,7 +1418,7 @@
       <c r="C15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1423,7 +1427,9 @@
       <c r="F15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="2:8" ht="22.05" customHeight="1">
       <c r="B16" s="17" t="s">
@@ -1432,7 +1438,7 @@
       <c r="C16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1441,7 +1447,9 @@
       <c r="F16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="22.05" customHeight="1">
       <c r="B17" s="17" t="s">
@@ -1450,7 +1458,7 @@
       <c r="C17" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="26" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1459,7 +1467,9 @@
       <c r="F17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="22.05" customHeight="1">
       <c r="B18" s="17" t="s">
@@ -1468,7 +1478,7 @@
       <c r="C18" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="26" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1477,7 +1487,9 @@
       <c r="F18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="22.05" customHeight="1">
       <c r="B19" s="17" t="s">
@@ -1486,11 +1498,11 @@
       <c r="C19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>13</v>
@@ -1504,7 +1516,7 @@
       <c r="C20" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="26" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -1522,7 +1534,7 @@
       <c r="C21" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="26" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -1531,7 +1543,9 @@
       <c r="F21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="22.05" customHeight="1">
       <c r="B22" s="17" t="s">
@@ -1540,7 +1554,7 @@
       <c r="C22" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="26" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1558,7 +1572,7 @@
       <c r="C23" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1576,7 +1590,7 @@
       <c r="C24" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -1594,7 +1608,7 @@
       <c r="C25" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="26" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -1612,7 +1626,7 @@
       <c r="C26" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1630,7 +1644,7 @@
       <c r="C27" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1648,7 +1662,7 @@
       <c r="C28" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -1666,7 +1680,7 @@
       <c r="C29" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1684,7 +1698,7 @@
       <c r="C30" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="26" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -1702,7 +1716,7 @@
       <c r="C31" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1720,7 +1734,7 @@
       <c r="C32" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="26" t="s">
         <v>57</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -1738,7 +1752,7 @@
       <c r="C33" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -1756,7 +1770,7 @@
       <c r="C34" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="26" t="s">
         <v>59</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -1774,7 +1788,7 @@
       <c r="C35" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="26" t="s">
         <v>60</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -1792,7 +1806,7 @@
       <c r="C36" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -1810,7 +1824,7 @@
       <c r="C37" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="26" t="s">
         <v>62</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -1828,7 +1842,7 @@
       <c r="C38" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="26" t="s">
         <v>63</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -1846,7 +1860,7 @@
       <c r="C39" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -1864,7 +1878,7 @@
       <c r="C40" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="26" t="s">
         <v>65</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -1882,7 +1896,7 @@
       <c r="C41" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -1900,7 +1914,7 @@
       <c r="C42" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="26" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -1918,7 +1932,7 @@
       <c r="C43" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="26" t="s">
         <v>68</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -1936,7 +1950,7 @@
       <c r="C44" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="26" t="s">
         <v>69</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -1954,7 +1968,7 @@
       <c r="C45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="26" t="s">
         <v>70</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -1972,7 +1986,7 @@
       <c r="C46" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="26" t="s">
         <v>71</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -1990,7 +2004,7 @@
       <c r="C47" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="26" t="s">
         <v>72</v>
       </c>
       <c r="E47" s="4" t="s">
@@ -2008,7 +2022,7 @@
       <c r="C48" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -2027,7 +2041,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="16">
         <f>SUM(G3:G12)</f>
-        <v>2.8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="22.05" customHeight="1"/>
@@ -2133,13 +2147,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="49.95" customHeight="1">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="2:6" ht="27" customHeight="1">
       <c r="B2" s="24" t="s">
@@ -2266,22 +2280,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:7" ht="27.75" customHeight="1">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="2:7" ht="22.05" customHeight="1">
       <c r="B3" s="3" t="s">

</xml_diff>

<commit_message>
docs(sprint): Add Sprint_2 kanban board
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F02A4-DEC2-4132-8ED1-7D282C990325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE4376-1D7A-4149-9816-1FFCF268FE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Dropdown Keys - DO NOT DELETE" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'RECORD BOOK'!$B$1:$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="75">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Add input/output adapters for future UI expansion (e.g., GUI, web)</t>
-  </si>
-  <si>
-    <t>Implement use cases for starting a new game, saving/loading, quitting</t>
   </si>
   <si>
     <t>Implement use cases for player actions (move, interact, inventory, etc.)</t>
@@ -1123,10 +1120,10 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H51"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1176,7 +1173,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>29</v>
@@ -1196,7 +1193,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>30</v>
@@ -1216,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>31</v>
@@ -1236,7 +1233,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
@@ -1256,7 +1253,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>32</v>
@@ -1276,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>33</v>
@@ -1296,10 +1293,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -1316,13 +1313,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>12</v>
@@ -1336,13 +1333,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>12</v>
@@ -1356,13 +1353,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>12</v>
@@ -1376,13 +1373,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>13</v>
@@ -1396,13 +1393,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>14</v>
@@ -1416,13 +1413,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>12</v>
@@ -1436,13 +1433,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>12</v>
@@ -1456,13 +1453,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>12</v>
@@ -1476,13 +1473,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>13</v>
@@ -1496,7 +1493,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>42</v>
@@ -1514,31 +1511,33 @@
         <v>8</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="G20" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="21" spans="2:7" ht="22.05" customHeight="1">
       <c r="B21" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F21" s="17" t="s">
         <v>13</v>
@@ -1552,169 +1551,187 @@
         <v>8</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="22.05" customHeight="1">
       <c r="B23" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="12"/>
+      <c r="G23" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="22.05" customHeight="1">
       <c r="B24" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="25" spans="2:7" ht="22.05" customHeight="1">
       <c r="B25" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:7" ht="22.05" customHeight="1">
       <c r="B26" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="12"/>
+      <c r="G26" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="22.05" customHeight="1">
       <c r="B27" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="22.05" customHeight="1">
       <c r="B28" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F28" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="22.05" customHeight="1">
       <c r="B29" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="12"/>
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:7" ht="22.05" customHeight="1">
       <c r="B30" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="22.05" customHeight="1">
       <c r="B31" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>56</v>
@@ -1729,10 +1746,10 @@
     </row>
     <row r="32" spans="2:7" ht="22.05" customHeight="1">
       <c r="B32" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>57</v>
@@ -1747,10 +1764,10 @@
     </row>
     <row r="33" spans="2:7" ht="22.05" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>58</v>
@@ -1768,7 +1785,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>59</v>
@@ -1786,7 +1803,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>60</v>
@@ -1795,7 +1812,7 @@
         <v>19</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="12"/>
     </row>
@@ -1804,7 +1821,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="26" t="s">
         <v>61</v>
@@ -1813,16 +1830,16 @@
         <v>19</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="2:7" ht="22.05" customHeight="1">
+    <row r="37" spans="2:7" ht="21.6" customHeight="1">
       <c r="B37" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>62</v>
@@ -1831,16 +1848,16 @@
         <v>19</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G37" s="12"/>
     </row>
-    <row r="38" spans="2:7" ht="21.6" customHeight="1">
+    <row r="38" spans="2:7" ht="22.05" customHeight="1">
       <c r="B38" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>63</v>
@@ -1849,7 +1866,7 @@
         <v>19</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G38" s="12"/>
     </row>
@@ -1858,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>64</v>
@@ -1867,7 +1884,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G39" s="12"/>
     </row>
@@ -1876,7 +1893,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>65</v>
@@ -1885,16 +1902,16 @@
         <v>19</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="2:7" ht="22.05" customHeight="1">
       <c r="B41" s="17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>66</v>
@@ -1903,7 +1920,7 @@
         <v>19</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G41" s="12"/>
     </row>
@@ -1912,7 +1929,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>67</v>
@@ -1927,10 +1944,10 @@
     </row>
     <row r="43" spans="2:7" ht="22.05" customHeight="1">
       <c r="B43" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="26" t="s">
         <v>68</v>
@@ -1945,10 +1962,10 @@
     </row>
     <row r="44" spans="2:7" ht="22.05" customHeight="1">
       <c r="B44" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" s="26" t="s">
         <v>69</v>
@@ -1966,7 +1983,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>70</v>
@@ -1981,10 +1998,10 @@
     </row>
     <row r="46" spans="2:7" ht="22.05" customHeight="1">
       <c r="B46" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="26" t="s">
         <v>71</v>
@@ -2002,7 +2019,7 @@
         <v>11</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" s="26" t="s">
         <v>72</v>
@@ -2016,41 +2033,23 @@
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="2:7" ht="22.05" customHeight="1">
-      <c r="B48" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="2:7" ht="22.05" customHeight="1">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="16">
-        <f>SUM(G3:G12)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="22.05" customHeight="1"/>
-    <row r="51" spans="2:7" ht="22.05" customHeight="1"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="16">
+        <f>SUM(G3:G47)</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="49" ht="22.05" customHeight="1"/>
+    <row r="50" ht="22.05" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B48">
+  <conditionalFormatting sqref="B3:B47">
     <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Update">
       <formula>NOT(ISERROR(SEARCH("Update",B3)))</formula>
     </cfRule>
@@ -2067,7 +2066,7 @@
       <formula>NOT(ISERROR(SEARCH("Research",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E48">
+  <conditionalFormatting sqref="E3:E47">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",E3)))</formula>
     </cfRule>
@@ -2084,7 +2083,7 @@
       <formula>NOT(ISERROR(SEARCH("In Progress",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F48">
+  <conditionalFormatting sqref="F3:F47">
     <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F3)))</formula>
     </cfRule>
@@ -2104,19 +2103,19 @@
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$D$4:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F48</xm:sqref>
+          <xm:sqref>F3:F47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F0F8AA5-B689-4426-BA33-6C1D47615340}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B48</xm:sqref>
+          <xm:sqref>B3:B47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B4C2DC5-C50B-4F79-B003-80EA0FBD9D80}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$F$4:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E48</xm:sqref>
+          <xm:sqref>E3:E47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat(world): Implement Room utilies and display world
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE4376-1D7A-4149-9816-1FFCF268FE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2031D-1D1C-40BC-A152-D1ABE75382AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -1122,8 +1122,8 @@
   </sheetPr>
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1617,7 +1617,7 @@
         <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>13</v>
@@ -1637,7 +1637,7 @@
         <v>51</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>13</v>
@@ -1657,7 +1657,7 @@
         <v>52</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>13</v>
@@ -1677,7 +1677,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F28" s="17" t="s">
         <v>13</v>
@@ -1697,7 +1697,7 @@
         <v>54</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>13</v>
@@ -1717,7 +1717,7 @@
         <v>55</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
docs(report): Small change in kanban board for sprint 2 and backlog
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2031D-1D1C-40BC-A152-D1ABE75382AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398CFEA-04F7-4C59-9FE4-BC63B74218D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Dropdown Keys - DO NOT DELETE" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ARCHIVE!$B$1:$G$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'RECORD BOOK'!$B$1:$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="76">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Define Backlog for the entire project</t>
+  </si>
+  <si>
+    <t>Disaply world</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1123,10 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H50"/>
+  <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1634,13 +1637,13 @@
         <v>73</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26" s="12">
         <v>2</v>
@@ -1654,10 +1657,10 @@
         <v>73</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>13</v>
@@ -1674,7 +1677,7 @@
         <v>73</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>20</v>
@@ -1683,7 +1686,7 @@
         <v>13</v>
       </c>
       <c r="G28" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="22.05" customHeight="1">
@@ -1694,7 +1697,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>20</v>
@@ -1703,7 +1706,7 @@
         <v>13</v>
       </c>
       <c r="G29" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="22.05" customHeight="1">
@@ -1714,7 +1717,7 @@
         <v>73</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>20</v>
@@ -1723,7 +1726,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="22.05" customHeight="1">
@@ -1734,25 +1737,27 @@
         <v>73</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="12"/>
+      <c r="G31" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="22.05" customHeight="1">
       <c r="B32" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>19</v>
@@ -1764,13 +1769,13 @@
     </row>
     <row r="33" spans="2:7" ht="22.05" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>19</v>
@@ -1788,7 +1793,7 @@
         <v>73</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>19</v>
@@ -1806,13 +1811,13 @@
         <v>73</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="12"/>
     </row>
@@ -1824,17 +1829,17 @@
         <v>73</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="2:7" ht="21.6" customHeight="1">
+    <row r="37" spans="2:7" ht="22.05" customHeight="1">
       <c r="B37" s="17" t="s">
         <v>8</v>
       </c>
@@ -1842,31 +1847,31 @@
         <v>73</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G37" s="12"/>
     </row>
-    <row r="38" spans="2:7" ht="22.05" customHeight="1">
+    <row r="38" spans="2:7" ht="21.6" customHeight="1">
       <c r="B38" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G38" s="12"/>
     </row>
@@ -1878,13 +1883,13 @@
         <v>73</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" s="12"/>
     </row>
@@ -1896,31 +1901,31 @@
         <v>73</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="2:7" ht="22.05" customHeight="1">
       <c r="B41" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" s="12"/>
     </row>
@@ -1932,7 +1937,7 @@
         <v>73</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>19</v>
@@ -1944,13 +1949,13 @@
     </row>
     <row r="43" spans="2:7" ht="22.05" customHeight="1">
       <c r="B43" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>19</v>
@@ -1962,13 +1967,13 @@
     </row>
     <row r="44" spans="2:7" ht="22.05" customHeight="1">
       <c r="B44" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>19</v>
@@ -1986,7 +1991,7 @@
         <v>73</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>19</v>
@@ -1998,13 +2003,13 @@
     </row>
     <row r="46" spans="2:7" ht="22.05" customHeight="1">
       <c r="B46" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>19</v>
@@ -2022,7 +2027,7 @@
         <v>73</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>19</v>
@@ -2033,23 +2038,41 @@
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="2:7" ht="22.05" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="16">
-        <f>SUM(G3:G47)</f>
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="49" ht="22.05" customHeight="1"/>
-    <row r="50" ht="22.05" customHeight="1"/>
+      <c r="B48" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="2:7" ht="22.05" customHeight="1">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="16">
+        <f>SUM(G3:G48)</f>
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="22.05" customHeight="1"/>
+    <row r="51" spans="2:7" ht="22.05" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B47">
+  <conditionalFormatting sqref="B3:B48">
     <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Update">
       <formula>NOT(ISERROR(SEARCH("Update",B3)))</formula>
     </cfRule>
@@ -2066,7 +2089,7 @@
       <formula>NOT(ISERROR(SEARCH("Research",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E47">
+  <conditionalFormatting sqref="E3:E48">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",E3)))</formula>
     </cfRule>
@@ -2083,7 +2106,7 @@
       <formula>NOT(ISERROR(SEARCH("In Progress",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F47">
+  <conditionalFormatting sqref="F3:F48">
     <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F3)))</formula>
     </cfRule>
@@ -2103,19 +2126,19 @@
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$D$4:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F47</xm:sqref>
+          <xm:sqref>F3:F48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F0F8AA5-B689-4426-BA33-6C1D47615340}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B47</xm:sqref>
+          <xm:sqref>B3:B48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B4C2DC5-C50B-4F79-B003-80EA0FBD9D80}">
           <x14:formula1>
             <xm:f>'Dropdown Keys - DO NOT DELETE'!$F$4:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E47</xm:sqref>
+          <xm:sqref>E3:E48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
docs(sprint): Add sprint 3 sheet
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398CFEA-04F7-4C59-9FE4-BC63B74218D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AFA9A5-1D1E-4427-A1A2-1EA52F4FA3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -239,9 +239,6 @@
     <t>Implement structure/object placement (buildings, dungeons, items)</t>
   </si>
   <si>
-    <t>Implement deterministic world generation using seeds</t>
-  </si>
-  <si>
     <t>Write tests for world generation consistency</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>Implement basic AI or NPC logic (if applicable)</t>
   </si>
   <si>
-    <t>Implement combat or challenge mechanics (if part of the design)</t>
-  </si>
-  <si>
     <t>Implement scoring, progression, or achievement systems</t>
   </si>
   <si>
@@ -297,6 +291,12 @@
   </si>
   <si>
     <t>Disaply world</t>
+  </si>
+  <si>
+    <t>Implement Enemy movement and combact system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement combat or challenge mechanics </t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
   </sheetPr>
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1176,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>29</v>
@@ -1196,7 +1196,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>30</v>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>31</v>
@@ -1236,7 +1236,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
@@ -1256,7 +1256,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>32</v>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>33</v>
@@ -1296,10 +1296,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -1316,7 +1316,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>34</v>
@@ -1336,7 +1336,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>35</v>
@@ -1356,7 +1356,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>45</v>
@@ -1376,7 +1376,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>36</v>
@@ -1396,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>37</v>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>38</v>
@@ -1436,7 +1436,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>39</v>
@@ -1456,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>40</v>
@@ -1476,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>41</v>
@@ -1496,25 +1496,27 @@
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="G19" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="22.05" customHeight="1">
       <c r="B20" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>43</v>
@@ -1534,7 +1536,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>46</v>
@@ -1554,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>47</v>
@@ -1574,7 +1576,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>48</v>
@@ -1594,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>49</v>
@@ -1614,7 +1616,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>50</v>
@@ -1634,10 +1636,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>73</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>20</v>
@@ -1654,19 +1656,19 @@
         <v>8</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="22.05" customHeight="1">
@@ -1674,7 +1676,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>52</v>
@@ -1694,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>53</v>
@@ -1714,7 +1716,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>54</v>
@@ -1734,7 +1736,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>55</v>
@@ -1751,85 +1753,93 @@
     </row>
     <row r="32" spans="2:7" ht="22.05" customHeight="1">
       <c r="B32" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="12"/>
+      <c r="G32" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:7" ht="22.05" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>57</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="12"/>
+      <c r="G33" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="2:7" ht="22.05" customHeight="1">
       <c r="B34" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="12"/>
+      <c r="G34" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="2:7" ht="22.05" customHeight="1">
       <c r="B35" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="12"/>
+      <c r="G35" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="2:7" ht="22.05" customHeight="1">
       <c r="B36" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>19</v>
@@ -1844,28 +1854,30 @@
         <v>8</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="12"/>
+      <c r="G37" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="21.6" customHeight="1">
       <c r="B38" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>19</v>
@@ -1873,17 +1885,19 @@
       <c r="F38" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="12"/>
+      <c r="G38" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="22.05" customHeight="1">
       <c r="B39" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>19</v>
@@ -1898,10 +1912,10 @@
         <v>7</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>19</v>
@@ -1916,10 +1930,10 @@
         <v>7</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>19</v>
@@ -1934,10 +1948,10 @@
         <v>10</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>19</v>
@@ -1952,10 +1966,10 @@
         <v>10</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>19</v>
@@ -1970,10 +1984,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>19</v>
@@ -1988,10 +2002,10 @@
         <v>9</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>19</v>
@@ -2006,10 +2020,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>19</v>
@@ -2024,10 +2038,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>19</v>
@@ -2042,10 +2056,10 @@
         <v>11</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>19</v>
@@ -2063,7 +2077,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="16">
         <f>SUM(G3:G48)</f>
-        <v>33.5</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="22.05" customHeight="1"/>

</xml_diff>

<commit_message>
docs(sprint): Update kanban board for end of sprint 3
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AFA9A5-1D1E-4427-A1A2-1EA52F4FA3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E66B17-40CC-4CF8-AE10-71EDB9E6B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -1125,8 +1125,8 @@
   </sheetPr>
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1502,7 +1502,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>13</v>
@@ -1662,7 +1662,7 @@
         <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>13</v>
@@ -1782,7 +1782,7 @@
         <v>57</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>13</v>
@@ -1802,7 +1802,7 @@
         <v>58</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>13</v>
@@ -1822,7 +1822,7 @@
         <v>74</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>13</v>
@@ -1860,7 +1860,7 @@
         <v>75</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
docs(sprint): Add kanbab board for the completed fourth sprint
</commit_message>
<xml_diff>
--- a/docs/boards/Backlog.xlsx
+++ b/docs/boards/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E66B17-40CC-4CF8-AE10-71EDB9E6B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4F140E-8FE0-460B-AC6A-F9B7C4641DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA5D6E8E-4F9F-4292-B407-0BB176AAE353}"/>
   </bookViews>
@@ -248,9 +248,6 @@
     <t>Implement inventory system and item management</t>
   </si>
   <si>
-    <t>Implement basic AI or NPC logic (if applicable)</t>
-  </si>
-  <si>
     <t>Implement scoring, progression, or achievement systems</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Set up integration tests for game loop and world generation</t>
   </si>
   <si>
-    <t>Implement property-based tests for procedural systems</t>
-  </si>
-  <si>
     <t>Perform manual playtesting and bug tracking</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
     <t>Add diagrams and visual aids to docs (architecture, workflows)</t>
   </si>
   <si>
-    <t>Document sprint reviews, retrospectives, and major decisions</t>
-  </si>
-  <si>
     <t>Refine CLI or UI for usability and clarity</t>
   </si>
   <si>
@@ -293,10 +284,19 @@
     <t>Disaply world</t>
   </si>
   <si>
-    <t>Implement Enemy movement and combact system</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement combat or challenge mechanics </t>
+  </si>
+  <si>
+    <t>Implement Enemy  combact system</t>
+  </si>
+  <si>
+    <t>Implement Enemy  movement system in prolog</t>
+  </si>
+  <si>
+    <t>Refactor view to use monads</t>
+  </si>
+  <si>
+    <t>Implement state history with Monad</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
   </sheetPr>
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1176,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>29</v>
@@ -1196,7 +1196,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>30</v>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>31</v>
@@ -1236,7 +1236,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
@@ -1256,7 +1256,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>32</v>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>33</v>
@@ -1296,10 +1296,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -1316,7 +1316,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>34</v>
@@ -1336,7 +1336,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>35</v>
@@ -1356,7 +1356,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>45</v>
@@ -1376,7 +1376,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>36</v>
@@ -1396,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>37</v>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>38</v>
@@ -1436,7 +1436,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>39</v>
@@ -1456,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>40</v>
@@ -1476,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>41</v>
@@ -1496,7 +1496,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>42</v>
@@ -1516,7 +1516,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>43</v>
@@ -1536,7 +1536,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>46</v>
@@ -1556,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>47</v>
@@ -1576,7 +1576,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>48</v>
@@ -1596,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>49</v>
@@ -1616,7 +1616,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>50</v>
@@ -1636,10 +1636,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>20</v>
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>51</v>
@@ -1676,7 +1676,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>52</v>
@@ -1696,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>53</v>
@@ -1716,7 +1716,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>54</v>
@@ -1736,7 +1736,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>55</v>
@@ -1756,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>56</v>
@@ -1776,7 +1776,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>57</v>
@@ -1796,7 +1796,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>58</v>
@@ -1816,10 +1816,10 @@
         <v>8</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>20</v>
@@ -1828,7 +1828,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="22.05" customHeight="1">
@@ -1836,28 +1836,30 @@
         <v>8</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="G36" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="22.05" customHeight="1">
       <c r="B37" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="26" t="s">
         <v>71</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>20</v>
@@ -1869,128 +1871,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="21.6" customHeight="1">
+    <row r="38" spans="2:7" ht="22.05" customHeight="1">
       <c r="B38" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="22.05" customHeight="1">
       <c r="B39" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="12"/>
-    </row>
-    <row r="40" spans="2:7" ht="22.05" customHeight="1">
+        <v>14</v>
+      </c>
+      <c r="G39" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="21.6" customHeight="1">
       <c r="B40" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="12"/>
+      <c r="G40" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="22.05" customHeight="1">
       <c r="B41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="12"/>
+      <c r="G41" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="2:7" ht="22.05" customHeight="1">
       <c r="B42" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="12"/>
+      <c r="G42" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="22.05" customHeight="1">
       <c r="B43" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="12"/>
+      <c r="G43" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="44" spans="2:7" ht="22.05" customHeight="1">
       <c r="B44" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F44" s="17" t="s">
         <v>14</v>
@@ -1999,16 +2011,16 @@
     </row>
     <row r="45" spans="2:7" ht="22.05" customHeight="1">
       <c r="B45" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F45" s="17" t="s">
         <v>14</v>
@@ -2020,13 +2032,13 @@
         <v>9</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>14</v>
@@ -2038,36 +2050,40 @@
         <v>11</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="12"/>
+      <c r="G47" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="48" spans="2:7" ht="22.05" customHeight="1">
       <c r="B48" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F48" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="12"/>
+      <c r="G48" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="2:7" ht="22.05" customHeight="1">
       <c r="B49" s="11"/>
@@ -2077,7 +2093,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="16">
         <f>SUM(G3:G48)</f>
-        <v>46.5</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="22.05" customHeight="1"/>

</xml_diff>